<commit_message>
commit WRN8IMB remaining code
</commit_message>
<xml_diff>
--- a/src/main/resources/documents/WRN8IMBConstruction.xlsx
+++ b/src/main/resources/documents/WRN8IMBConstruction.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="46">
   <si>
     <t>(Do Not Modify) Account</t>
   </si>
@@ -163,6 +163,18 @@
   </si>
   <si>
     <t>Test8IMB20240917SITE70376</t>
+  </si>
+  <si>
+    <t>Test8IMB20240918SITE70170</t>
+  </si>
+  <si>
+    <t>Test8IMB20240918SITE23569</t>
+  </si>
+  <si>
+    <t>Test8IMB20240918SITE52252</t>
+  </si>
+  <si>
+    <t>Test8IMB20240918SITE63629</t>
   </si>
 </sst>
 </file>
@@ -651,7 +663,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="D2" s="5" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>12</v>

</xml_diff>